<commit_message>
added eurofer low carbon roadmap data
</commit_message>
<xml_diff>
--- a/data/scenariolibrary.xlsx
+++ b/data/scenariolibrary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD1D04-2DA3-2D44-9403-74C5356ECC0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7E2B80-99F9-A142-8322-099B7BCE0494}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="620" windowWidth="25720" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>References</t>
   </si>
@@ -86,13 +86,58 @@
   </si>
   <si>
     <t>100% charcoal</t>
+  </si>
+  <si>
+    <t>EUROFER 1990</t>
+  </si>
+  <si>
+    <t>EUFOFER 2030_Base</t>
+  </si>
+  <si>
+    <t>EUFOFER 2030_Max-No CCS</t>
+  </si>
+  <si>
+    <t>EUFOFER 2030_Max-CCS</t>
+  </si>
+  <si>
+    <t>EUROFER 2030_Economic</t>
+  </si>
+  <si>
+    <t>EUFOFER 2050_Base</t>
+  </si>
+  <si>
+    <t>EUFOFER 2050_Max-No CCS</t>
+  </si>
+  <si>
+    <t>EUFOFER 2050_Max-CCS</t>
+  </si>
+  <si>
+    <t>EUROFER 2050_Economic</t>
+  </si>
+  <si>
+    <t>Combined BF + EAF production</t>
+  </si>
+  <si>
+    <t>EUROFER 2010</t>
+  </si>
+  <si>
+    <t>0% to CCS (rollout begins in 2030)</t>
+  </si>
+  <si>
+    <t>% to geological sequestration</t>
+  </si>
+  <si>
+    <t>electricity included</t>
+  </si>
+  <si>
+    <t>electricity included; assumes full decarbonization of electricity by 2050</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +149,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,12 +181,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,17 +468,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.5" customWidth="1"/>
     <col min="5" max="5" width="33.5" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" customWidth="1"/>
@@ -525,8 +578,121 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D7" s="2"/>
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates to IEAGHG scenario
rechecking of emission and energy data based on source
</commit_message>
<xml_diff>
--- a/data/scenariolibrary.xlsx
+++ b/data/scenariolibrary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7E2B80-99F9-A142-8322-099B7BCE0494}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F37ACA-EAE2-4B41-ACDC-89FA77755906}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="620" windowWidth="25720" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>References</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>electricity included; assumes full decarbonization of electricity by 2050</t>
+  </si>
+  <si>
+    <t>ieaghg-reference</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>BF production</t>
+  </si>
+  <si>
+    <t>electricity partially co-generated from fluegases</t>
   </si>
 </sst>
 </file>
@@ -468,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -694,6 +706,23 @@
         <v>34</v>
       </c>
     </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added medium-complexity steel model
</commit_message>
<xml_diff>
--- a/data/scenariolibrary.xlsx
+++ b/data/scenariolibrary.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F37ACA-EAE2-4B41-ACDC-89FA77755906}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="620" windowWidth="25720" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="615" windowWidth="25725" windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="steel" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
   <si>
     <t>References</t>
   </si>
@@ -143,12 +142,75 @@
   </si>
   <si>
     <t>electricity partially co-generated from fluegases</t>
+  </si>
+  <si>
+    <t>global-BF-base</t>
+  </si>
+  <si>
+    <t>global-EAF-base</t>
+  </si>
+  <si>
+    <t>EU-BF-base</t>
+  </si>
+  <si>
+    <t>EU-EAF-base</t>
+  </si>
+  <si>
+    <t>USA-BF-base</t>
+  </si>
+  <si>
+    <t>USA-EAF-base</t>
+  </si>
+  <si>
+    <t>China-BF-base</t>
+  </si>
+  <si>
+    <t>China-EAF-base</t>
+  </si>
+  <si>
+    <t>India-BF-base</t>
+  </si>
+  <si>
+    <t>Japan-BF-base</t>
+  </si>
+  <si>
+    <t>Russia-BF-base</t>
+  </si>
+  <si>
+    <t>SouthKorea-BF-base</t>
+  </si>
+  <si>
+    <t>India-EAF-base</t>
+  </si>
+  <si>
+    <t>Japan-EAF-base</t>
+  </si>
+  <si>
+    <t>Russia-EAF-base</t>
+  </si>
+  <si>
+    <t>SouthKorea-EAF-base</t>
+  </si>
+  <si>
+    <t>coal, waste plastics</t>
+  </si>
+  <si>
+    <t>coal, natural gas</t>
+  </si>
+  <si>
+    <t>electricity mix</t>
+  </si>
+  <si>
+    <t>BF+BOF</t>
+  </si>
+  <si>
+    <t>EAF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -479,25 +541,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5" customWidth="1"/>
-    <col min="5" max="5" width="33.5" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" customWidth="1"/>
-    <col min="7" max="7" width="37.5" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -520,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -531,7 +596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -548,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -562,7 +627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -576,7 +641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -590,10 +655,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
@@ -601,10 +669,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
@@ -612,10 +683,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>29</v>
       </c>
@@ -623,10 +697,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
       </c>
@@ -634,7 +711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -648,10 +725,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
@@ -659,10 +739,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>29</v>
       </c>
@@ -670,10 +753,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
       </c>
@@ -681,7 +767,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -695,10 +781,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
       </c>
@@ -706,7 +795,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -721,6 +810,230 @@
       </c>
       <c r="E17" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
meso-level steel production data
</commit_message>
<xml_diff>
--- a/data/scenariolibrary.xlsx
+++ b/data/scenariolibrary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA2D85E-2C16-1640-B3DC-BBADB5E21CAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="615" windowWidth="25725" windowHeight="16380"/>
+    <workbookView xWindow="2760" yWindow="620" windowWidth="25720" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="steel" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="61">
   <si>
     <t>References</t>
   </si>
@@ -205,12 +206,15 @@
   </si>
   <si>
     <t>EAF</t>
+  </si>
+  <si>
+    <t>china-HeEtAl2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,28 +545,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -585,7 +589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -596,7 +600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -613,7 +617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -627,7 +631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -641,7 +645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -655,7 +659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -669,7 +673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -683,7 +687,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -697,7 +701,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -711,7 +715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -725,7 +729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -739,7 +743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -753,7 +757,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -767,7 +771,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -781,7 +785,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -795,7 +799,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -812,7 +816,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -826,7 +830,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -840,7 +844,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -854,7 +858,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -868,7 +872,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -882,7 +886,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -896,7 +900,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -910,7 +914,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -924,7 +928,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -938,7 +942,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -952,7 +956,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -966,7 +970,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -980,7 +984,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -994,7 +998,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1034,6 +1038,20 @@
       </c>
       <c r="D33" s="2" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
numbers suck but trying to fix them
</commit_message>
<xml_diff>
--- a/data/scenariolibrary.xlsx
+++ b/data/scenariolibrary.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CA9210-19F7-EA46-A4F9-3FC4D2EF866E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="615" windowWidth="25725" windowHeight="16380"/>
+    <workbookView xWindow="2760" yWindow="620" windowWidth="18980" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="steel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
   <si>
     <t>References</t>
   </si>
@@ -207,9 +208,6 @@
     <t>EAF</t>
   </si>
   <si>
-    <t>china-HeEtAl2017</t>
-  </si>
-  <si>
     <t>He et al 2017</t>
   </si>
   <si>
@@ -223,12 +221,36 @@
   </si>
   <si>
     <t>Kuramochi 2016</t>
+  </si>
+  <si>
+    <t>EU-BF-I</t>
+  </si>
+  <si>
+    <t>EU-BF-C</t>
+  </si>
+  <si>
+    <t>EU-BF-M</t>
+  </si>
+  <si>
+    <t>EU-BF-F</t>
+  </si>
+  <si>
+    <t>China-BF-I</t>
+  </si>
+  <si>
+    <t>China-BF-C</t>
+  </si>
+  <si>
+    <t>China-BF-M</t>
+  </si>
+  <si>
+    <t>China-BF-F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,28 +581,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -603,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -614,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -631,7 +653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -645,7 +667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -659,7 +681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -673,7 +695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -687,7 +709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -701,7 +723,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -715,7 +737,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -729,7 +751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -743,7 +765,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -757,7 +779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -771,7 +793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -785,7 +807,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -799,7 +821,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -813,7 +835,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -830,7 +852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -844,7 +866,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -858,10 +880,10 @@
         <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -875,10 +897,10 @@
         <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -892,7 +914,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -906,10 +928,10 @@
         <v>58</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -923,10 +945,10 @@
         <v>58</v>
       </c>
       <c r="G23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -940,7 +962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -954,7 +976,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -968,10 +990,10 @@
         <v>59</v>
       </c>
       <c r="G26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -985,7 +1007,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -999,7 +1021,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1013,7 +1035,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1027,7 +1049,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1041,7 +1063,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1055,7 +1077,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1069,18 +1091,44 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>